<commit_message>
feat(insurance) add partial paied
</commit_message>
<xml_diff>
--- a/bybit/work/insurance/相互保1.01新增翻译.xlsx
+++ b/bybit/work/insurance/相互保1.01新增翻译.xlsx
@@ -1159,8 +1159,8 @@
   <sheetPr/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="4"/>
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>33</v>
@@ -1371,6 +1371,9 @@
         <v>34</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
@@ -1424,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="18" spans="1:4">
+    <row r="20" ht="18" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>43</v>
@@ -1433,8 +1436,11 @@
         <v>44</v>
       </c>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" ht="18.35" spans="1:4">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="18.35" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>45</v>
@@ -1444,6 +1450,9 @@
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="18.35" spans="2:5">

</xml_diff>

<commit_message>
feat(insurance) insurance 切换symbol 为 coin
</commit_message>
<xml_diff>
--- a/bybit/work/insurance/相互保1.01新增翻译.xlsx
+++ b/bybit/work/insurance/相互保1.01新增翻译.xlsx
@@ -192,10 +192,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -215,6 +215,36 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,6 +258,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -237,17 +291,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -259,88 +342,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -349,9 +350,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,25 +372,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +456,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,7 +486,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,127 +534,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,6 +584,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -614,30 +638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -652,8 +652,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,148 +677,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1156,8 +1156,8 @@
   <sheetPr/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="4"/>
@@ -1490,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" ht="18.35" spans="2:5">
       <c r="B25" t="s">
         <v>53</v>
       </c>

</xml_diff>